<commit_message>
made VAD excel a bit colorful for better clarity of data
</commit_message>
<xml_diff>
--- a/Results/Results_VAD.xlsx
+++ b/Results/Results_VAD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29421"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOKUS\LESS_2\SE_26\src\LESSGuaidanceForRequirementFormalization\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOKUS\LESS_2\SE_26\src\LESS\LESSGuaidanceForRequirementFormalization\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{972275EB-8473-49DC-9F2B-4BF37C480866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C340E7EA-A656-45C8-9B68-EAADC00BA375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="1" activeTab="3" xr2:uid="{34E2BE8E-85C9-4BDF-A9B0-7DEAF13743E9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{34E2BE8E-85C9-4BDF-A9B0-7DEAF13743E9}"/>
   </bookViews>
   <sheets>
     <sheet name="NL_TO_LESS" sheetId="1" r:id="rId1"/>
@@ -31,16 +31,17 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
   <si>
     <t>LESS Requirement Generation</t>
   </si>
@@ -812,39 +813,7 @@
     <t>Grammar in NLP</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">22/28 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(line 10 was not considered because it is semantically wrong)</t>
-    </r>
-  </si>
-  <si>
     <t>17 (~77%)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">15/28
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Lines 2,10,11,13,14 not considered)</t>
-    </r>
   </si>
   <si>
     <t>12 (80%)</t>
@@ -871,22 +840,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">22/28 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Line 10 and 11 not considered because they are semantically wrong)</t>
-    </r>
-  </si>
-  <si>
     <t>20 (90%)</t>
   </si>
   <si>
@@ -935,13 +888,76 @@
   </si>
   <si>
     <t>15 (68%)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22 (out of 28 in GT)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(line 10 was not considered because it is semantically wrong)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">15 (out of 28 in GT)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Lines 2,10,11,13,14 not considered)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22 (out of 28 in GT)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Line 10 and 11 not considered because they are semantically wrong)</t>
+    </r>
+  </si>
+  <si>
+    <t>28 (Correct Gen: 19)</t>
+  </si>
+  <si>
+    <t>28 (Correct Gen: 12)</t>
+  </si>
+  <si>
+    <t>28 (Correct Gen: 18)</t>
+  </si>
+  <si>
+    <t>28 (Correct Gen: 22, Incorrect: 6)</t>
+  </si>
+  <si>
+    <t>28 (Correct Gen: 15, Incorrect: 13)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1068,7 +1084,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1323,13 +1339,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1354,15 +1396,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1373,157 +1406,193 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1841,472 +1910,508 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AAD88-F198-489C-B36B-918A39BD4411}">
-  <dimension ref="B1:L35"/>
+  <dimension ref="B1:M34"/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="64" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="44.28515625" customWidth="1"/>
-    <col min="7" max="7" width="39.42578125" customWidth="1"/>
-    <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="33.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" customWidth="1"/>
-    <col min="12" max="12" width="113.28515625" customWidth="1"/>
+    <col min="3" max="4" width="32.3828125" customWidth="1"/>
+    <col min="5" max="5" width="37.69140625" customWidth="1"/>
+    <col min="6" max="6" width="24.3046875" customWidth="1"/>
+    <col min="7" max="7" width="44.3046875" customWidth="1"/>
+    <col min="8" max="8" width="39.3828125" customWidth="1"/>
+    <col min="9" max="9" width="32" customWidth="1"/>
+    <col min="10" max="10" width="33.69140625" customWidth="1"/>
+    <col min="11" max="11" width="30.3828125" customWidth="1"/>
+    <col min="12" max="12" width="23.3828125" customWidth="1"/>
+    <col min="13" max="13" width="113.3046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15">
-      <c r="B1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="L1" s="15" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="M1" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="15">
-      <c r="B2" s="58" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-    </row>
-    <row r="3" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B3" s="23" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+    </row>
+    <row r="3" spans="2:13" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="59" t="s">
+      <c r="D3" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="62" t="s">
+      <c r="F3" s="57"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="63"/>
-    </row>
-    <row r="4" spans="2:12" ht="30.75">
-      <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25" t="s">
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+      <c r="K3" s="61"/>
+    </row>
+    <row r="4" spans="2:13" ht="29.15" x14ac:dyDescent="0.4">
+      <c r="B4" s="55"/>
+      <c r="C4" s="54"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="F4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="G4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="H4" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="I4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="J4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="K4" s="26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="15">
-      <c r="B5" s="18" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B5" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E5" s="19">
         <v>19</v>
       </c>
-      <c r="E5" s="22">
-        <v>0</v>
-      </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
-      <c r="G5" s="22">
+      <c r="F5" s="19">
+        <v>0</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+      <c r="H5" s="19">
         <v>3</v>
       </c>
-      <c r="H5" s="22">
+      <c r="I5" s="19">
         <v>3</v>
       </c>
-      <c r="I5" s="22">
+      <c r="J5" s="19">
         <v>1</v>
       </c>
-      <c r="J5" s="22">
+      <c r="K5" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="15">
-      <c r="B6" s="18"/>
-      <c r="C6" s="21" t="s">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B6" s="41"/>
+      <c r="C6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="18">
         <v>12</v>
       </c>
-      <c r="E6" s="21">
-        <v>0</v>
-      </c>
-      <c r="F6" s="21">
-        <v>0</v>
-      </c>
-      <c r="G6" s="21">
+      <c r="F6" s="18">
+        <v>0</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0</v>
+      </c>
+      <c r="H6" s="18">
         <v>4</v>
       </c>
-      <c r="H6" s="21">
+      <c r="I6" s="18">
         <v>8</v>
       </c>
-      <c r="I6" s="21">
+      <c r="J6" s="18">
         <v>2</v>
       </c>
-      <c r="J6" s="22">
+      <c r="K6" s="19">
         <v>2</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="15">
-      <c r="B7" s="18"/>
-      <c r="C7" s="21" t="s">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B7" s="41"/>
+      <c r="C7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E7" s="18">
         <v>18</v>
       </c>
-      <c r="E7" s="21">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21">
+      <c r="F7" s="18">
+        <v>0</v>
+      </c>
+      <c r="G7" s="18">
+        <v>0</v>
+      </c>
+      <c r="H7" s="18">
         <v>4</v>
       </c>
-      <c r="H7" s="21">
+      <c r="I7" s="18">
         <v>3</v>
       </c>
-      <c r="I7" s="21">
+      <c r="J7" s="18">
         <v>1</v>
       </c>
-      <c r="J7" s="22">
+      <c r="K7" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="15">
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="29"/>
-    </row>
-    <row r="9" spans="2:12" ht="45.75">
-      <c r="B9" s="31" t="s">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="23"/>
+    </row>
+    <row r="9" spans="2:13" ht="36.9" x14ac:dyDescent="0.4">
+      <c r="B9" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="18">
         <v>21</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="F9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="G9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="H9" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="I9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="30" t="s">
+      <c r="J9" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="74.650000000000006" customHeight="1">
-      <c r="B10" s="18"/>
-      <c r="C10" s="21" t="s">
+      <c r="K9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" ht="74.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="41"/>
+      <c r="C10" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" s="18">
         <v>15</v>
       </c>
-      <c r="E10" s="21">
-        <v>0</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="18">
+        <v>0</v>
+      </c>
+      <c r="G10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="H10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="I10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="K10" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="45.75">
-      <c r="B11" s="18"/>
-      <c r="C11" s="21" t="s">
+    <row r="11" spans="2:13" ht="36.9" x14ac:dyDescent="0.4">
+      <c r="B11" s="41"/>
+      <c r="C11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="18">
         <v>21</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="F11" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="G11" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="H11" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="I11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I11" s="21">
-        <v>0</v>
-      </c>
-      <c r="J11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="56.25" customHeight="1">
-      <c r="B12" s="18"/>
-      <c r="C12" s="36" t="s">
+      <c r="J11" s="18">
+        <v>0</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="41"/>
+      <c r="C12" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="F12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="38" t="s">
+      <c r="G12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="36" t="s">
+      <c r="H12" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="I12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="36" t="s">
+      <c r="J12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="J12" s="36" t="s">
+      <c r="K12" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="14" t="s">
+      <c r="M12" s="14" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="15"/>
-    <row r="14" spans="2:12" ht="14.65" customHeight="1">
-      <c r="B14" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-    </row>
-    <row r="15" spans="2:12" ht="15">
-      <c r="B15" s="54" t="s">
+    <row r="14" spans="2:13" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B15" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-    </row>
-    <row r="16" spans="2:12" ht="15">
-      <c r="B16" s="51" t="s">
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B16" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="52"/>
-      <c r="D16" s="53" t="s">
+      <c r="C16" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="77"/>
+      <c r="E16" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="53" t="s">
+      <c r="F16" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="53" t="s">
+      <c r="G16" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="53" t="s">
+      <c r="H16" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="53" t="s">
+      <c r="I16" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="53" t="s">
+      <c r="J16" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="J16" s="53" t="s">
+      <c r="K16" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="53" t="s">
+      <c r="L16" s="35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="30.75">
-      <c r="B17" s="18"/>
-      <c r="C17" s="19" t="s">
+    <row r="17" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B17" s="41"/>
+      <c r="C17" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="79"/>
+      <c r="E17" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="21">
-        <v>0</v>
-      </c>
-      <c r="F17" s="21">
-        <v>0</v>
-      </c>
-      <c r="G17" s="21">
-        <v>0</v>
-      </c>
-      <c r="H17" s="19" t="s">
+      <c r="F17" s="18">
+        <v>0</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0</v>
+      </c>
+      <c r="H17" s="18">
+        <v>0</v>
+      </c>
+      <c r="I17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="J17" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J17" s="21">
-        <v>0</v>
-      </c>
-      <c r="K17" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" ht="30.75">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19" t="s">
+      <c r="K17" s="18">
+        <v>0</v>
+      </c>
+      <c r="L17" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B18" s="41"/>
+      <c r="C18" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="79"/>
+      <c r="E18" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="21">
-        <v>0</v>
-      </c>
-      <c r="F18" s="21">
-        <v>0</v>
-      </c>
-      <c r="G18" s="21">
-        <v>0</v>
-      </c>
-      <c r="H18" s="19" t="s">
+      <c r="F18" s="18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="J18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="J18" s="21">
-        <v>0</v>
-      </c>
-      <c r="K18" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" ht="30.75">
-      <c r="B19" s="18"/>
-      <c r="C19" s="19" t="s">
+      <c r="K18" s="18">
+        <v>0</v>
+      </c>
+      <c r="L18" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B19" s="41"/>
+      <c r="C19" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="79"/>
+      <c r="E19" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="21">
-        <v>0</v>
-      </c>
-      <c r="F19" s="21">
-        <v>0</v>
-      </c>
-      <c r="G19" s="21">
-        <v>0</v>
-      </c>
-      <c r="H19" s="19" t="s">
+      <c r="F19" s="18">
+        <v>0</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
+      <c r="H19" s="18">
+        <v>0</v>
+      </c>
+      <c r="I19" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="J19" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="J19" s="21">
-        <v>0</v>
-      </c>
-      <c r="K19" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" ht="15">
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="49"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="50"/>
-    </row>
-    <row r="21" spans="2:11" ht="15">
+      <c r="K19" s="18">
+        <v>0</v>
+      </c>
+      <c r="L19" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B20" s="32"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
@@ -2317,315 +2422,341 @@
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
-    </row>
-    <row r="22" spans="2:11" ht="14.65" customHeight="1">
-      <c r="B22" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-    </row>
-    <row r="23" spans="2:11" ht="15">
-      <c r="B23" s="55" t="s">
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="2:12" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="51"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="51"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B23" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="57"/>
-    </row>
-    <row r="24" spans="2:11" ht="15">
-      <c r="B24" s="51" t="s">
+      <c r="C23" s="46"/>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
+      <c r="L23" s="47"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B24" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53" t="s">
+      <c r="C24" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="77"/>
+      <c r="E24" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="F24" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F24" s="53" t="s">
+      <c r="G24" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="53" t="s">
+      <c r="H24" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="53" t="s">
+      <c r="I24" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="53" t="s">
+      <c r="J24" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="J24" s="53" t="s">
+      <c r="K24" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="K24" s="53" t="s">
+      <c r="L24" s="35" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="30.75">
-      <c r="B25" s="18"/>
-      <c r="C25" s="19" t="s">
+    <row r="25" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B25" s="41"/>
+      <c r="C25" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="79"/>
+      <c r="E25" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="21">
-        <v>0</v>
-      </c>
-      <c r="F25" s="21">
-        <v>0</v>
-      </c>
-      <c r="G25" s="21">
-        <v>0</v>
-      </c>
-      <c r="H25" s="21">
-        <v>0</v>
-      </c>
-      <c r="I25" s="21">
-        <v>0</v>
-      </c>
-      <c r="J25" s="21">
-        <v>0</v>
-      </c>
-      <c r="K25" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" ht="30.75">
-      <c r="B26" s="18"/>
-      <c r="C26" s="19" t="s">
+      <c r="F25" s="18">
+        <v>0</v>
+      </c>
+      <c r="G25" s="18">
+        <v>0</v>
+      </c>
+      <c r="H25" s="18">
+        <v>0</v>
+      </c>
+      <c r="I25" s="18">
+        <v>0</v>
+      </c>
+      <c r="J25" s="18">
+        <v>0</v>
+      </c>
+      <c r="K25" s="18">
+        <v>0</v>
+      </c>
+      <c r="L25" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B26" s="41"/>
+      <c r="C26" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="79"/>
+      <c r="E26" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="21">
-        <v>0</v>
-      </c>
-      <c r="F26" s="21">
-        <v>0</v>
-      </c>
-      <c r="G26" s="21">
-        <v>0</v>
-      </c>
-      <c r="H26" s="21">
-        <v>0</v>
-      </c>
-      <c r="I26" s="21">
-        <v>0</v>
-      </c>
-      <c r="J26" s="21">
-        <v>0</v>
-      </c>
-      <c r="K26" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" ht="30.75">
-      <c r="B27" s="18"/>
-      <c r="C27" s="19" t="s">
+      <c r="F26" s="18">
+        <v>0</v>
+      </c>
+      <c r="G26" s="18">
+        <v>0</v>
+      </c>
+      <c r="H26" s="18">
+        <v>0</v>
+      </c>
+      <c r="I26" s="18">
+        <v>0</v>
+      </c>
+      <c r="J26" s="18">
+        <v>0</v>
+      </c>
+      <c r="K26" s="18">
+        <v>0</v>
+      </c>
+      <c r="L26" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B27" s="41"/>
+      <c r="C27" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="79"/>
+      <c r="E27" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="21">
-        <v>0</v>
-      </c>
-      <c r="F27" s="21">
-        <v>0</v>
-      </c>
-      <c r="G27" s="21">
-        <v>0</v>
-      </c>
-      <c r="H27" s="21">
-        <v>0</v>
-      </c>
-      <c r="I27" s="21">
-        <v>0</v>
-      </c>
-      <c r="J27" s="21">
-        <v>0</v>
-      </c>
-      <c r="K27" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" ht="15"/>
-    <row r="29" spans="2:11" ht="15">
-      <c r="B29" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="47"/>
-    </row>
-    <row r="30" spans="2:11" ht="15">
-      <c r="B30" s="55" t="s">
+      <c r="F27" s="18">
+        <v>0</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0</v>
+      </c>
+      <c r="H27" s="18">
+        <v>0</v>
+      </c>
+      <c r="I27" s="18">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18">
+        <v>0</v>
+      </c>
+      <c r="K27" s="18">
+        <v>0</v>
+      </c>
+      <c r="L27" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B29" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
+      <c r="K29" s="44"/>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B30" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="57"/>
-    </row>
-    <row r="31" spans="2:11" ht="15">
-      <c r="B31" s="40" t="s">
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="47"/>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B31" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="81"/>
+      <c r="E31" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="F31" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="G31" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="G31" s="40" t="s">
+      <c r="H31" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H31" s="40" t="s">
+      <c r="I31" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="40" t="s">
+      <c r="J31" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="J31" s="40" t="s">
+      <c r="K31" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="2:11" ht="30.75">
-      <c r="B32" s="35" t="s">
+    <row r="32" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B32" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="22">
-        <v>0</v>
-      </c>
-      <c r="E32" s="22">
-        <v>0</v>
-      </c>
-      <c r="F32" s="22">
-        <v>0</v>
-      </c>
-      <c r="G32" s="22">
-        <v>0</v>
-      </c>
-      <c r="H32" s="22">
-        <v>0</v>
-      </c>
-      <c r="I32" s="22">
-        <v>0</v>
-      </c>
-      <c r="J32" s="21" t="s">
+      <c r="D32" s="83"/>
+      <c r="E32" s="19">
+        <v>0</v>
+      </c>
+      <c r="F32" s="19">
+        <v>0</v>
+      </c>
+      <c r="G32" s="19">
+        <v>0</v>
+      </c>
+      <c r="H32" s="19">
+        <v>0</v>
+      </c>
+      <c r="I32" s="19">
+        <v>0</v>
+      </c>
+      <c r="J32" s="19">
+        <v>0</v>
+      </c>
+      <c r="K32" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="30.75">
-      <c r="B33" s="43"/>
-      <c r="C33" s="22" t="s">
+    <row r="33" spans="2:11" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B33" s="49"/>
+      <c r="C33" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="22">
-        <v>0</v>
-      </c>
-      <c r="E33" s="22">
-        <v>0</v>
-      </c>
-      <c r="F33" s="22">
-        <v>0</v>
-      </c>
-      <c r="G33" s="22">
-        <v>0</v>
-      </c>
-      <c r="H33" s="21" t="s">
+      <c r="D33" s="83"/>
+      <c r="E33" s="19">
+        <v>0</v>
+      </c>
+      <c r="F33" s="19">
+        <v>0</v>
+      </c>
+      <c r="G33" s="19">
+        <v>0</v>
+      </c>
+      <c r="H33" s="19">
+        <v>0</v>
+      </c>
+      <c r="I33" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="I33" s="21" t="s">
+      <c r="J33" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="J33" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="30.75">
-      <c r="B34" s="44"/>
-      <c r="C34" s="22" t="s">
+      <c r="K33" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="26.15" x14ac:dyDescent="0.4">
+      <c r="B34" s="50"/>
+      <c r="C34" s="82" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="22">
-        <v>0</v>
-      </c>
-      <c r="E34" s="22">
-        <v>0</v>
-      </c>
-      <c r="F34" s="22">
-        <v>0</v>
-      </c>
-      <c r="G34" s="22">
-        <v>0</v>
-      </c>
-      <c r="H34" s="22">
-        <v>0</v>
-      </c>
-      <c r="I34" s="22">
-        <v>0</v>
-      </c>
-      <c r="J34" s="21" t="s">
+      <c r="D34" s="83"/>
+      <c r="E34" s="19">
+        <v>0</v>
+      </c>
+      <c r="F34" s="19">
+        <v>0</v>
+      </c>
+      <c r="G34" s="19">
+        <v>0</v>
+      </c>
+      <c r="H34" s="19">
+        <v>0</v>
+      </c>
+      <c r="I34" s="19">
+        <v>0</v>
+      </c>
+      <c r="J34" s="19">
+        <v>0</v>
+      </c>
+      <c r="K34" s="18" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15"/>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B29:J29"/>
-    <mergeCell ref="B30:J30"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B22:K22"/>
-    <mergeCell ref="B14:K14"/>
-    <mergeCell ref="B15:K15"/>
-    <mergeCell ref="B23:K23"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B2:J2"/>
+  <mergeCells count="31">
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B2:K2"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="H3:K3"/>
     <mergeCell ref="B9:B12"/>
     <mergeCell ref="B16:B19"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B29:K29"/>
+    <mergeCell ref="B30:K30"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2634,49 +2765,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03285090-925E-4318-9A54-5659E6D310C9}">
-  <dimension ref="C1:J16"/>
+  <dimension ref="C3:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.69140625" customWidth="1"/>
+    <col min="4" max="4" width="18.69140625" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="38.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.69140625" customWidth="1"/>
+    <col min="7" max="7" width="23.3046875" customWidth="1"/>
+    <col min="8" max="8" width="28.53515625" customWidth="1"/>
+    <col min="9" max="9" width="23.53515625" customWidth="1"/>
+    <col min="10" max="10" width="20.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" ht="15"/>
-    <row r="2" spans="3:10" ht="15"/>
-    <row r="3" spans="3:10" ht="15">
-      <c r="C3" s="45" t="s">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C3" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="47"/>
-    </row>
-    <row r="4" spans="3:10" ht="14.65" customHeight="1">
-      <c r="C4" s="67" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="44"/>
+    </row>
+    <row r="4" spans="3:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="69" t="s">
+      <c r="E4" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="67" t="s">
+      <c r="F4" s="65" t="s">
         <v>75</v>
       </c>
       <c r="G4" s="64" t="s">
@@ -2684,108 +2813,100 @@
       </c>
       <c r="H4" s="64"/>
       <c r="I4" s="64"/>
-      <c r="J4" s="41"/>
-    </row>
-    <row r="5" spans="3:10" ht="14.65" customHeight="1">
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="71" t="s">
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="3:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="71" t="s">
+      <c r="H5" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="71" t="s">
+      <c r="I5" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="J5" s="71" t="s">
+      <c r="J5" s="38" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="3:10" ht="29.25" customHeight="1">
-      <c r="C6" s="42" t="s">
+    <row r="6" spans="3:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="G6" s="19">
+        <v>5</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0</v>
+      </c>
+      <c r="I6" s="19">
+        <v>0</v>
+      </c>
+      <c r="J6" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="37" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="49"/>
+      <c r="D7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="22">
-        <v>5</v>
-      </c>
-      <c r="H6" s="22">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22">
-        <v>0</v>
-      </c>
-      <c r="J6" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" ht="36.950000000000003" customHeight="1">
-      <c r="C7" s="43"/>
-      <c r="D7" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="G7" s="19">
+        <v>2</v>
+      </c>
+      <c r="H7" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="I7" s="19">
+        <v>0</v>
+      </c>
+      <c r="J7" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="37" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="50"/>
+      <c r="D8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="22">
-        <v>2</v>
-      </c>
-      <c r="H7" s="27" t="s">
+      <c r="G8" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="I7" s="22">
-        <v>0</v>
-      </c>
-      <c r="J7" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" ht="36.950000000000003" customHeight="1">
-      <c r="C8" s="44"/>
-      <c r="D8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="G8" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="H8" s="22">
-        <v>0</v>
-      </c>
-      <c r="I8" s="22">
-        <v>0</v>
-      </c>
-      <c r="J8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" ht="15"/>
-    <row r="10" spans="3:10" ht="15"/>
-    <row r="11" spans="3:10" ht="15"/>
-    <row r="12" spans="3:10" ht="15"/>
-    <row r="13" spans="3:10" ht="15"/>
-    <row r="14" spans="3:10" ht="15"/>
-    <row r="15" spans="3:10" ht="15"/>
-    <row r="16" spans="3:10" ht="15"/>
+      <c r="H8" s="19">
+        <v>0</v>
+      </c>
+      <c r="I8" s="19">
+        <v>0</v>
+      </c>
+      <c r="J8" s="19">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="C6:C8"/>
@@ -2808,42 +2929,42 @@
       <selection activeCell="C1" sqref="C1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="29.15234375" customWidth="1"/>
+    <col min="4" max="4" width="33.84375" customWidth="1"/>
+    <col min="5" max="5" width="13.84375" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.3046875" customWidth="1"/>
+    <col min="9" max="9" width="13.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10">
-      <c r="C1" s="17" t="s">
+    <row r="1" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C1" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="3:10">
-      <c r="C2" s="16" t="s">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.4">
+      <c r="C2" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="4" spans="3:10">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
@@ -2851,13 +2972,13 @@
         <v>4</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
         <v>15</v>
@@ -2865,7 +2986,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="3:10">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C6" s="1" t="s">
         <v>80</v>
       </c>
@@ -2874,7 +2995,7 @@
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="3:10">
+    <row r="7" spans="3:10" x14ac:dyDescent="0.4">
       <c r="C7" s="3"/>
       <c r="D7" s="4" t="s">
         <v>18</v>
@@ -2893,59 +3014,59 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2638F1-068A-4418-89AB-4E730123006C}">
-  <dimension ref="B2:I21"/>
+  <dimension ref="B2:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.15234375" customWidth="1"/>
+    <col min="3" max="3" width="29.69140625" customWidth="1"/>
+    <col min="4" max="4" width="31.15234375" customWidth="1"/>
+    <col min="5" max="5" width="27.3046875" customWidth="1"/>
+    <col min="6" max="6" width="30.3046875" customWidth="1"/>
+    <col min="7" max="7" width="27.15234375" customWidth="1"/>
+    <col min="8" max="8" width="22.69140625" customWidth="1"/>
+    <col min="9" max="9" width="40.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9">
-      <c r="B2" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-    </row>
-    <row r="3" spans="2:9" ht="15">
-      <c r="B3" s="39" t="s">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B2" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-    </row>
-    <row r="4" spans="2:9" ht="14.65" customHeight="1">
-      <c r="B4" s="67" t="s">
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+    </row>
+    <row r="4" spans="2:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="73" t="s">
-        <v>92</v>
-      </c>
-      <c r="E4" s="67" t="s">
+      <c r="D4" s="72" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="65" t="s">
         <v>75</v>
       </c>
       <c r="F4" s="64" t="s">
@@ -2955,103 +3076,98 @@
       <c r="H4" s="64"/>
       <c r="I4" s="64"/>
     </row>
-    <row r="5" spans="2:9" ht="29.1" customHeight="1">
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="65" t="s">
+    <row r="5" spans="2:9" ht="29.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="65" t="s">
+      <c r="G5" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="66" t="s">
+      <c r="H5" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="72" t="s">
+      <c r="I5" s="39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B6" s="63" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="17">
+        <v>22</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="17">
+        <v>4</v>
+      </c>
+      <c r="G6" s="17">
+        <v>10</v>
+      </c>
+      <c r="H6" s="17">
+        <v>0</v>
+      </c>
+      <c r="I6" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="49"/>
+      <c r="C7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="17">
+        <v>15</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="17">
+        <v>2</v>
+      </c>
+      <c r="G7" s="17">
+        <v>3</v>
+      </c>
+      <c r="H7" s="17">
+        <v>1</v>
+      </c>
+      <c r="I7" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="50"/>
+      <c r="C8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="17">
+        <v>22</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="15">
-      <c r="B6" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="20">
-        <v>22</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="20">
+      <c r="F8" s="17">
+        <v>2</v>
+      </c>
+      <c r="G8" s="17">
         <v>4</v>
       </c>
-      <c r="G6" s="20">
-        <v>10</v>
-      </c>
-      <c r="H6" s="20">
-        <v>0</v>
-      </c>
-      <c r="I6" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="14.65" customHeight="1">
-      <c r="B7" s="43"/>
-      <c r="C7" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="20">
-        <v>15</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="F7" s="20">
+      <c r="H8" s="17">
         <v>2</v>
       </c>
-      <c r="G7" s="20">
-        <v>3</v>
-      </c>
-      <c r="H7" s="20">
-        <v>1</v>
-      </c>
-      <c r="I7" s="20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="14.65" customHeight="1">
-      <c r="B8" s="44"/>
-      <c r="C8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="20">
-        <v>22</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="F8" s="20">
-        <v>2</v>
-      </c>
-      <c r="G8" s="20">
-        <v>4</v>
-      </c>
-      <c r="H8" s="20">
-        <v>2</v>
-      </c>
-      <c r="I8" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="15"/>
-    <row r="11" spans="2:9" ht="15"/>
-    <row r="12" spans="2:9" ht="15"/>
-    <row r="20" ht="15"/>
-    <row r="21" ht="15"/>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="B6:B8"/>
@@ -3076,31 +3192,31 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.65"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.3046875" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" customWidth="1"/>
+    <col min="4" max="4" width="41.69140625" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B1" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="2:5">
-      <c r="B2" s="16" t="s">
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
+      <c r="B2" s="70" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-    </row>
-    <row r="4" spans="2:5">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B4" s="10" t="s">
         <v>3</v>
       </c>
@@ -3108,13 +3224,13 @@
         <v>4</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
         <v>15</v>
@@ -3122,7 +3238,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>80</v>
       </c>
@@ -3131,7 +3247,7 @@
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Added details on the VAD case study
</commit_message>
<xml_diff>
--- a/Results/Results_VAD.xlsx
+++ b/Results/Results_VAD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29421"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOKUS\LESS_2\SE_26\src\LESS\LESSGuaidanceForRequirementFormalization\Results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FOKUS\LESS_2\SE_26\src\LESSGuaidanceForRequirementFormalization\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C340E7EA-A656-45C8-9B68-EAADC00BA375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="13_ncr:1_{D54DE534-4750-415D-96FF-0924464667CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D510301-FFA8-4FDE-ADCE-E56E855D5272}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{34E2BE8E-85C9-4BDF-A9B0-7DEAF13743E9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" firstSheet="3" activeTab="3" xr2:uid="{34E2BE8E-85C9-4BDF-A9B0-7DEAF13743E9}"/>
   </bookViews>
   <sheets>
     <sheet name="NL_TO_LESS" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,140 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="103">
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Results are best of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3 runs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. 
+All RUN details and results are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">confidential
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Please refer to EGAS case study for in-depth analysis of results</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Evaluation dataset (ground truth): </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> N/A
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Total NL-LESS pair in Eval. set: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">35
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Total NL requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> given to model for generation: 28
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FSL Examples: 7</t>
+    </r>
+  </si>
   <si>
     <t>LESS Requirement Generation</t>
   </si>
@@ -789,6 +912,90 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Runs: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The entries here are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>best results from 3 runs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for all models
+Detailed results from all runs are organised per model in location: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF4472C4"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N/A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ground Truth:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For corresponding models, LESS requirements generated correctly by that model was provided as LESS input to generate test cases
+Ground truth is organised in each model folder as "Deterministic". The same LESS requirement given to individual models to generate test cases were given to a python script to generate test cases, this is then considerd as base line. 
+All locations in table below</t>
+    </r>
+  </si>
+  <si>
     <t>LESS to Test Case Generation</t>
   </si>
   <si>
@@ -813,9 +1020,41 @@
     <t>Grammar in NLP</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">22/28 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(line 10 was not considered because it is semantically wrong)</t>
+    </r>
+  </si>
+  <si>
     <t>17 (~77%)</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">15/28
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Lines 2,10,11,13,14 not considered)</t>
+    </r>
+  </si>
+  <si>
     <t>12 (80%)</t>
   </si>
   <si>
@@ -837,6 +1076,22 @@
         <scheme val="minor"/>
       </rPr>
       <t>(1 only incompleteness other 2 incompleteness + misclass)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">22/28 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Line 10 and 11 not considered because they are semantically wrong)</t>
     </r>
   </si>
   <si>
@@ -872,6 +1127,88 @@
     <t>Hallucinated outputs</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Runs: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The entries here are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>best results from 3 runs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for all models
+Detailed results from all runs are organised per model in location:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> n/a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ground Truth:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> For corresponding models, NL equivalent of the LESS requirements generated correctly by that model was provided as NL input to generate test cases
+Ground truth is organised in each model folder as "Deterministic". </t>
+    </r>
+  </si>
+  <si>
     <t>NLP to Test Case Generation</t>
   </si>
   <si>
@@ -888,76 +1225,13 @@
   </si>
   <si>
     <t>15 (68%)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">22 (out of 28 in GT)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(line 10 was not considered because it is semantically wrong)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">15 (out of 28 in GT)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Lines 2,10,11,13,14 not considered)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">22 (out of 28 in GT)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(Line 10 and 11 not considered because they are semantically wrong)</t>
-    </r>
-  </si>
-  <si>
-    <t>28 (Correct Gen: 19)</t>
-  </si>
-  <si>
-    <t>28 (Correct Gen: 12)</t>
-  </si>
-  <si>
-    <t>28 (Correct Gen: 18)</t>
-  </si>
-  <si>
-    <t>28 (Correct Gen: 22, Incorrect: 6)</t>
-  </si>
-  <si>
-    <t>28 (Correct Gen: 15, Incorrect: 13)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1017,8 +1291,42 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF4472C4"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1083,8 +1391,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1341,10 +1660,43 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -1354,10 +1706,28 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -1366,12 +1736,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="22" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1440,165 +1811,181 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="19" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="21" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="25" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="22" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="23" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="1" builtinId="23"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1910,853 +2297,819 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79AAD88-F198-489C-B36B-918A39BD4411}">
-  <dimension ref="B1:M34"/>
+  <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="64" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView zoomScale="64" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="4" width="32.3828125" customWidth="1"/>
-    <col min="5" max="5" width="37.69140625" customWidth="1"/>
-    <col min="6" max="6" width="24.3046875" customWidth="1"/>
-    <col min="7" max="7" width="44.3046875" customWidth="1"/>
-    <col min="8" max="8" width="39.3828125" customWidth="1"/>
-    <col min="9" max="9" width="32" customWidth="1"/>
-    <col min="10" max="10" width="33.69140625" customWidth="1"/>
-    <col min="11" max="11" width="30.3828125" customWidth="1"/>
-    <col min="12" max="12" width="23.3828125" customWidth="1"/>
-    <col min="13" max="13" width="113.3046875" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="33.7109375" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.42578125" customWidth="1"/>
+    <col min="12" max="12" width="113.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="M1" s="15" t="s">
+    <row r="1" spans="2:12" ht="67.5" customHeight="1">
+      <c r="B1" s="73" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="75"/>
+    </row>
+    <row r="2" spans="2:12" ht="94.5" customHeight="1">
+      <c r="B2" s="70" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B2" s="53" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="72"/>
+    </row>
+    <row r="3" spans="2:12" ht="15">
+      <c r="B3" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-    </row>
-    <row r="3" spans="2:13" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="55" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="L3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="54" t="s">
+    </row>
+    <row r="4" spans="2:12" ht="15">
+      <c r="B4" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="74" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="56" t="s">
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+    </row>
+    <row r="5" spans="2:12" ht="14.65" customHeight="1">
+      <c r="B5" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="57"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="60" t="s">
+      <c r="C5" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="61"/>
-    </row>
-    <row r="4" spans="2:13" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="B4" s="55"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="20" t="s">
+      <c r="D5" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="E5" s="54"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="58"/>
+    </row>
+    <row r="6" spans="2:12" ht="30.75">
+      <c r="B6" s="52"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="E6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="25" t="s">
+      <c r="F6" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="G6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="H6" s="25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B5" s="41" t="s">
+      <c r="I6" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="J6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="19">
+    </row>
+    <row r="7" spans="2:12" ht="15">
+      <c r="B7" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="19">
         <v>19</v>
       </c>
-      <c r="F5" s="19">
-        <v>0</v>
-      </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
-      <c r="H5" s="19">
+      <c r="E7" s="19">
+        <v>0</v>
+      </c>
+      <c r="F7" s="19">
+        <v>0</v>
+      </c>
+      <c r="G7" s="19">
         <v>3</v>
       </c>
-      <c r="I5" s="19">
+      <c r="H7" s="19">
         <v>3</v>
       </c>
-      <c r="J5" s="19">
+      <c r="I7" s="19">
         <v>1</v>
       </c>
-      <c r="K5" s="19">
+      <c r="J7" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B6" s="41"/>
-      <c r="C6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="E6" s="18">
+    <row r="8" spans="2:12" ht="15">
+      <c r="B8" s="39"/>
+      <c r="C8" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="18">
         <v>12</v>
       </c>
-      <c r="F6" s="18">
-        <v>0</v>
-      </c>
-      <c r="G6" s="18">
-        <v>0</v>
-      </c>
-      <c r="H6" s="18">
+      <c r="E8" s="18">
+        <v>0</v>
+      </c>
+      <c r="F8" s="18">
+        <v>0</v>
+      </c>
+      <c r="G8" s="18">
         <v>4</v>
       </c>
-      <c r="I6" s="18">
+      <c r="H8" s="18">
         <v>8</v>
       </c>
-      <c r="J6" s="18">
+      <c r="I8" s="18">
         <v>2</v>
       </c>
-      <c r="K6" s="19">
+      <c r="J8" s="19">
         <v>2</v>
       </c>
-      <c r="M6" t="s">
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="15">
+      <c r="B9" s="39"/>
+      <c r="C9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="18">
+        <v>18</v>
+      </c>
+      <c r="E9" s="18">
+        <v>0</v>
+      </c>
+      <c r="F9" s="18">
+        <v>0</v>
+      </c>
+      <c r="G9" s="18">
+        <v>4</v>
+      </c>
+      <c r="H9" s="18">
+        <v>3</v>
+      </c>
+      <c r="I9" s="18">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="15">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="23"/>
+    </row>
+    <row r="11" spans="2:12" ht="45.75">
+      <c r="B11" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B7" s="41"/>
-      <c r="C7" s="18" t="s">
+      <c r="D11" s="18">
+        <v>21</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="74.650000000000006" customHeight="1">
+      <c r="B12" s="39"/>
+      <c r="C12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="D12" s="18">
+        <v>15</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="45.75">
+      <c r="B13" s="39"/>
+      <c r="C13" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="18">
+        <v>21</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="18">
+        <v>0</v>
+      </c>
+      <c r="J13" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" ht="56.25" customHeight="1">
+      <c r="B14" s="39"/>
+      <c r="C14" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="15"/>
+    <row r="16" spans="2:12" ht="14.65" customHeight="1">
+      <c r="B16" s="48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="48"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+    </row>
+    <row r="17" spans="2:11" ht="15">
+      <c r="B17" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+    </row>
+    <row r="18" spans="2:11" ht="15">
+      <c r="B18" s="87" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="30.75">
+      <c r="B19" s="39"/>
+      <c r="C19" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0</v>
+      </c>
+      <c r="F19" s="18">
+        <v>0</v>
+      </c>
+      <c r="G19" s="18">
+        <v>0</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J19" s="18">
+        <v>0</v>
+      </c>
+      <c r="K19" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="30.75">
+      <c r="B20" s="39"/>
+      <c r="C20" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="18">
-        <v>0</v>
-      </c>
-      <c r="G7" s="18">
-        <v>0</v>
-      </c>
-      <c r="H7" s="18">
-        <v>4</v>
-      </c>
-      <c r="I7" s="18">
-        <v>3</v>
-      </c>
-      <c r="J7" s="18">
-        <v>1</v>
-      </c>
-      <c r="K7" s="19">
+      <c r="D20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0</v>
+      </c>
+      <c r="F20" s="18">
+        <v>0</v>
+      </c>
+      <c r="G20" s="18">
+        <v>0</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="18">
+        <v>0</v>
+      </c>
+      <c r="K20" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="30.75">
+      <c r="B21" s="39"/>
+      <c r="C21" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="18">
+        <v>0</v>
+      </c>
+      <c r="F21" s="18">
+        <v>0</v>
+      </c>
+      <c r="G21" s="18">
+        <v>0</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="J21" s="18">
+        <v>0</v>
+      </c>
+      <c r="K21" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="15">
+      <c r="B22" s="32"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+    </row>
+    <row r="23" spans="2:11" ht="15">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="2:11" ht="14.65" customHeight="1">
+      <c r="B24" s="48" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="23"/>
-    </row>
-    <row r="9" spans="2:13" ht="36.9" x14ac:dyDescent="0.4">
-      <c r="B9" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="C24" s="48"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="48"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="48"/>
+    </row>
+    <row r="25" spans="2:11" ht="15">
+      <c r="B25" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
+      <c r="F25" s="44"/>
+      <c r="G25" s="44"/>
+      <c r="H25" s="44"/>
+      <c r="I25" s="44"/>
+      <c r="J25" s="44"/>
+      <c r="K25" s="45"/>
+    </row>
+    <row r="26" spans="2:11" ht="15">
+      <c r="B26" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="C26" s="33"/>
+      <c r="D26" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="30.75">
+      <c r="B27" s="39"/>
+      <c r="C27" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="18">
+        <v>0</v>
+      </c>
+      <c r="F27" s="18">
+        <v>0</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0</v>
+      </c>
+      <c r="H27" s="18">
+        <v>0</v>
+      </c>
+      <c r="I27" s="18">
+        <v>0</v>
+      </c>
+      <c r="J27" s="18">
+        <v>0</v>
+      </c>
+      <c r="K27" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="30.75">
+      <c r="B28" s="39"/>
+      <c r="C28" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0</v>
+      </c>
+      <c r="F28" s="18">
+        <v>0</v>
+      </c>
+      <c r="G28" s="18">
+        <v>0</v>
+      </c>
+      <c r="H28" s="18">
+        <v>0</v>
+      </c>
+      <c r="I28" s="18">
+        <v>0</v>
+      </c>
+      <c r="J28" s="18">
+        <v>0</v>
+      </c>
+      <c r="K28" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="30.75">
+      <c r="B29" s="39"/>
+      <c r="C29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="D29" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="18">
+        <v>0</v>
+      </c>
+      <c r="F29" s="18">
+        <v>0</v>
+      </c>
+      <c r="G29" s="18">
+        <v>0</v>
+      </c>
+      <c r="H29" s="18">
+        <v>0</v>
+      </c>
+      <c r="I29" s="18">
+        <v>0</v>
+      </c>
+      <c r="J29" s="18">
+        <v>0</v>
+      </c>
+      <c r="K29" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="15"/>
+    <row r="31" spans="2:11" ht="15">
+      <c r="B31" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="41"/>
+      <c r="J31" s="42"/>
+    </row>
+    <row r="32" spans="2:11" ht="15">
+      <c r="B32" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="44"/>
+      <c r="F32" s="44"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="44"/>
+      <c r="J32" s="45"/>
+    </row>
+    <row r="33" spans="2:10" ht="15">
+      <c r="B33" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="I33" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="J33" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="30.75">
+      <c r="B34" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" ht="74.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="41"/>
-      <c r="C10" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E10" s="18">
-        <v>15</v>
-      </c>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13" ht="36.9" x14ac:dyDescent="0.4">
-      <c r="B11" s="41"/>
-      <c r="C11" s="18" t="s">
+      <c r="C34" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="19">
+        <v>0</v>
+      </c>
+      <c r="E34" s="19">
+        <v>0</v>
+      </c>
+      <c r="F34" s="19">
+        <v>0</v>
+      </c>
+      <c r="G34" s="19">
+        <v>0</v>
+      </c>
+      <c r="H34" s="19">
+        <v>0</v>
+      </c>
+      <c r="I34" s="19">
+        <v>0</v>
+      </c>
+      <c r="J34" s="18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="30.75">
+      <c r="B35" s="46"/>
+      <c r="C35" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="18">
-        <v>21</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="18">
-        <v>0</v>
-      </c>
-      <c r="K11" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="41"/>
-      <c r="C12" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="I12" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="J12" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="M12" s="14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="51"/>
-      <c r="K14" s="51"/>
-      <c r="L14" s="51"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B15" s="52" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="52"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B16" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="I16" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="J16" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K16" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="L16" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B17" s="41"/>
-      <c r="C17" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="79"/>
-      <c r="E17" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="18">
-        <v>0</v>
-      </c>
-      <c r="G17" s="18">
-        <v>0</v>
-      </c>
-      <c r="H17" s="18">
-        <v>0</v>
-      </c>
-      <c r="I17" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="J17" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="K17" s="18">
-        <v>0</v>
-      </c>
-      <c r="L17" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B18" s="41"/>
-      <c r="C18" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" s="18">
-        <v>0</v>
-      </c>
-      <c r="G18" s="18">
-        <v>0</v>
-      </c>
-      <c r="H18" s="18">
-        <v>0</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="18">
-        <v>0</v>
-      </c>
-      <c r="L18" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B19" s="41"/>
-      <c r="C19" s="78" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="79"/>
-      <c r="E19" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="18">
-        <v>0</v>
-      </c>
-      <c r="G19" s="18">
-        <v>0</v>
-      </c>
-      <c r="H19" s="18">
-        <v>0</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="K19" s="18">
-        <v>0</v>
-      </c>
-      <c r="L19" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B20" s="32"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-    </row>
-    <row r="22" spans="2:12" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B22" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
-      <c r="I22" s="51"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B23" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
-      <c r="L23" s="47"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B24" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="77"/>
-      <c r="E24" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="I24" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="J24" s="35" t="s">
-        <v>49</v>
-      </c>
-      <c r="K24" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="L24" s="35" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B25" s="41"/>
-      <c r="C25" s="78" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="79"/>
-      <c r="E25" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="F25" s="18">
-        <v>0</v>
-      </c>
-      <c r="G25" s="18">
-        <v>0</v>
-      </c>
-      <c r="H25" s="18">
-        <v>0</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="18">
-        <v>0</v>
-      </c>
-      <c r="K25" s="18">
-        <v>0</v>
-      </c>
-      <c r="L25" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B26" s="41"/>
-      <c r="C26" s="78" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="79"/>
-      <c r="E26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="18">
-        <v>0</v>
-      </c>
-      <c r="G26" s="18">
-        <v>0</v>
-      </c>
-      <c r="H26" s="18">
-        <v>0</v>
-      </c>
-      <c r="I26" s="18">
-        <v>0</v>
-      </c>
-      <c r="J26" s="18">
-        <v>0</v>
-      </c>
-      <c r="K26" s="18">
-        <v>0</v>
-      </c>
-      <c r="L26" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B27" s="41"/>
-      <c r="C27" s="78" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="79"/>
-      <c r="E27" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="18">
-        <v>0</v>
-      </c>
-      <c r="G27" s="18">
-        <v>0</v>
-      </c>
-      <c r="H27" s="18">
-        <v>0</v>
-      </c>
-      <c r="I27" s="18">
-        <v>0</v>
-      </c>
-      <c r="J27" s="18">
-        <v>0</v>
-      </c>
-      <c r="K27" s="18">
-        <v>0</v>
-      </c>
-      <c r="L27" s="18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B29" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
-      <c r="K29" s="44"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B30" s="45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="46"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="46"/>
-      <c r="G30" s="46"/>
-      <c r="H30" s="46"/>
-      <c r="I30" s="46"/>
-      <c r="J30" s="46"/>
-      <c r="K30" s="47"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B31" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="80" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="81"/>
-      <c r="E31" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="H31" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="I31" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="J31" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="K31" s="30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="2:12" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B32" s="48" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="83"/>
-      <c r="E32" s="19">
-        <v>0</v>
-      </c>
-      <c r="F32" s="19">
-        <v>0</v>
-      </c>
-      <c r="G32" s="19">
-        <v>0</v>
-      </c>
-      <c r="H32" s="19">
-        <v>0</v>
-      </c>
-      <c r="I32" s="19">
-        <v>0</v>
-      </c>
-      <c r="J32" s="19">
-        <v>0</v>
-      </c>
-      <c r="K32" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B33" s="49"/>
-      <c r="C33" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="83"/>
-      <c r="E33" s="19">
-        <v>0</v>
-      </c>
-      <c r="F33" s="19">
-        <v>0</v>
-      </c>
-      <c r="G33" s="19">
-        <v>0</v>
-      </c>
-      <c r="H33" s="19">
-        <v>0</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="J33" s="18" t="s">
+      <c r="D35" s="19">
+        <v>0</v>
+      </c>
+      <c r="E35" s="19">
+        <v>0</v>
+      </c>
+      <c r="F35" s="19">
+        <v>0</v>
+      </c>
+      <c r="G35" s="19">
+        <v>0</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J35" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="30.75">
+      <c r="B36" s="47"/>
+      <c r="C36" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="19">
+        <v>0</v>
+      </c>
+      <c r="E36" s="19">
+        <v>0</v>
+      </c>
+      <c r="F36" s="19">
+        <v>0</v>
+      </c>
+      <c r="G36" s="19">
+        <v>0</v>
+      </c>
+      <c r="H36" s="19">
+        <v>0</v>
+      </c>
+      <c r="I36" s="19">
+        <v>0</v>
+      </c>
+      <c r="J36" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="K33" s="19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" ht="26.15" x14ac:dyDescent="0.4">
-      <c r="B34" s="50"/>
-      <c r="C34" s="82" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="83"/>
-      <c r="E34" s="19">
-        <v>0</v>
-      </c>
-      <c r="F34" s="19">
-        <v>0</v>
-      </c>
-      <c r="G34" s="19">
-        <v>0</v>
-      </c>
-      <c r="H34" s="19">
-        <v>0</v>
-      </c>
-      <c r="I34" s="19">
-        <v>0</v>
-      </c>
-      <c r="J34" s="19">
-        <v>0</v>
-      </c>
-      <c r="K34" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
+    </row>
+    <row r="37" spans="2:10" ht="15"/>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B8:J8"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B29:K29"/>
-    <mergeCell ref="B30:K30"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
+  <mergeCells count="20">
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B17:K17"/>
+    <mergeCell ref="B25:K25"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="B24:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2765,86 +3118,110 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03285090-925E-4318-9A54-5659E6D310C9}">
-  <dimension ref="C3:J8"/>
+  <dimension ref="C1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col min="3" max="3" width="25.69140625" customWidth="1"/>
-    <col min="4" max="4" width="18.69140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
-    <col min="6" max="6" width="38.69140625" customWidth="1"/>
-    <col min="7" max="7" width="23.3046875" customWidth="1"/>
-    <col min="8" max="8" width="28.53515625" customWidth="1"/>
-    <col min="9" max="9" width="23.53515625" customWidth="1"/>
-    <col min="10" max="10" width="20.53515625" customWidth="1"/>
+    <col min="6" max="6" width="38.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:10" x14ac:dyDescent="0.4">
-      <c r="C3" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="44"/>
-    </row>
-    <row r="4" spans="3:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="65" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="65" t="s">
+    <row r="1" spans="3:10" ht="71.25" customHeight="1">
+      <c r="C1" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="G4" s="64" t="s">
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
+    </row>
+    <row r="2" spans="3:10" ht="57" customHeight="1">
+      <c r="C2" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="79"/>
+    </row>
+    <row r="3" spans="3:10" ht="15">
+      <c r="C3" s="83" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="84"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="85"/>
+    </row>
+    <row r="4" spans="3:10" ht="14.65" customHeight="1">
+      <c r="C4" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
       <c r="J4" s="31"/>
     </row>
-    <row r="5" spans="3:10" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="I5" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="J5" s="38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="63" t="s">
-        <v>80</v>
+    <row r="5" spans="3:10" ht="14.65" customHeight="1">
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="29.25" customHeight="1">
+      <c r="C6" s="59" t="s">
+        <v>84</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G6" s="19">
         <v>5</v>
@@ -2859,22 +3236,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="3:10" ht="37" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C7" s="49"/>
+    <row r="7" spans="3:10" ht="36.950000000000003" customHeight="1">
+      <c r="C7" s="46"/>
       <c r="D7" s="17" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="G7" s="19">
         <v>2</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="I7" s="19">
         <v>0</v>
@@ -2883,19 +3260,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="3:10" ht="37" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="50"/>
+    <row r="8" spans="3:10" ht="36.950000000000003" customHeight="1">
+      <c r="C8" s="47"/>
       <c r="D8" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="G8" s="24" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="H8" s="19">
         <v>0</v>
@@ -2907,8 +3284,18 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="3:10" ht="15"/>
+    <row r="10" spans="3:10" ht="15"/>
+    <row r="11" spans="3:10" ht="15"/>
+    <row r="12" spans="3:10" ht="15"/>
+    <row r="13" spans="3:10" ht="15"/>
+    <row r="14" spans="3:10" ht="15"/>
+    <row r="15" spans="3:10" ht="15"/>
+    <row r="16" spans="3:10" ht="15"/>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C2:J2"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="G4:I4"/>
@@ -2929,76 +3316,76 @@
       <selection activeCell="C1" sqref="C1:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col min="3" max="3" width="29.15234375" customWidth="1"/>
-    <col min="4" max="4" width="33.84375" customWidth="1"/>
-    <col min="5" max="5" width="13.84375" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="16.3046875" customWidth="1"/>
-    <col min="9" max="9" width="13.53515625" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:10" x14ac:dyDescent="0.4">
-      <c r="C1" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
+    <row r="1" spans="3:10">
+      <c r="C1" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="3:10" x14ac:dyDescent="0.4">
-      <c r="C2" s="70" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
+    <row r="2" spans="3:10">
+      <c r="C2" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="4" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="3:10">
       <c r="C4" s="10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
       <c r="C5" s="7"/>
       <c r="D5" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="3:10">
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="3:10">
       <c r="C7" s="3"/>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
@@ -3014,170 +3401,203 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2638F1-068A-4418-89AB-4E730123006C}">
-  <dimension ref="B2:I8"/>
+  <dimension ref="B1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col min="2" max="2" width="38.15234375" customWidth="1"/>
-    <col min="3" max="3" width="29.69140625" customWidth="1"/>
-    <col min="4" max="4" width="31.15234375" customWidth="1"/>
-    <col min="5" max="5" width="27.3046875" customWidth="1"/>
-    <col min="6" max="6" width="30.3046875" customWidth="1"/>
-    <col min="7" max="7" width="27.15234375" customWidth="1"/>
-    <col min="8" max="8" width="22.69140625" customWidth="1"/>
-    <col min="9" max="9" width="40.69140625" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B2" s="51" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-    </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B3" s="71" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-    </row>
-    <row r="4" spans="2:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="65" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="65" t="s">
+    <row r="1" spans="2:9" ht="15"/>
+    <row r="2" spans="2:9" ht="50.25" customHeight="1">
+      <c r="B2" s="80" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="82"/>
+    </row>
+    <row r="3" spans="2:9" ht="70.5" customHeight="1">
+      <c r="B3" s="77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="79"/>
+    </row>
+    <row r="4" spans="2:9" ht="15">
+      <c r="B4" s="76" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+    </row>
+    <row r="5" spans="2:9" ht="15">
+      <c r="B5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="72" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4" s="65" t="s">
-        <v>75</v>
-      </c>
-      <c r="F4" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-    </row>
-    <row r="5" spans="2:9" ht="29.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B6" s="63" t="s">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+    </row>
+    <row r="6" spans="2:9" ht="14.65" customHeight="1">
+      <c r="B6" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="60" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="17">
-        <v>22</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="17">
-        <v>4</v>
-      </c>
-      <c r="G6" s="17">
-        <v>10</v>
-      </c>
-      <c r="H6" s="17">
-        <v>0</v>
-      </c>
-      <c r="I6" s="17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="49"/>
-      <c r="C7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="17">
-        <v>15</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" s="17">
-        <v>2</v>
-      </c>
-      <c r="G7" s="17">
-        <v>3</v>
-      </c>
-      <c r="H7" s="17">
-        <v>1</v>
-      </c>
-      <c r="I7" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="50"/>
+      <c r="G6" s="60"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="60"/>
+    </row>
+    <row r="7" spans="2:9" ht="29.1" customHeight="1">
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="15">
+      <c r="B8" s="59" t="s">
+        <v>84</v>
+      </c>
       <c r="C8" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="17">
         <v>22</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F8" s="17">
+        <v>4</v>
+      </c>
+      <c r="G8" s="17">
+        <v>10</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0</v>
+      </c>
+      <c r="I8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="14.65" customHeight="1">
+      <c r="B9" s="46"/>
+      <c r="C9" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="17">
+        <v>15</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="17">
         <v>2</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G9" s="17">
+        <v>3</v>
+      </c>
+      <c r="H9" s="17">
+        <v>1</v>
+      </c>
+      <c r="I9" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="14.65" customHeight="1">
+      <c r="B10" s="47"/>
+      <c r="C10" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="17">
+        <v>22</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="17">
+        <v>2</v>
+      </c>
+      <c r="G10" s="17">
         <v>4</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H10" s="17">
         <v>2</v>
       </c>
-      <c r="I8" s="17">
-        <v>0</v>
-      </c>
-    </row>
+      <c r="I10" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="15"/>
+    <row r="13" spans="2:9" ht="15"/>
+    <row r="14" spans="2:9" ht="15"/>
+    <row r="22" ht="15"/>
+    <row r="23" ht="15"/>
+    <row r="24" ht="15"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B6:B8"/>
+  <mergeCells count="10">
+    <mergeCell ref="B2:I2"/>
     <mergeCell ref="B3:I3"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="B4:I4"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3192,65 +3612,65 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
-    <col min="2" max="2" width="35.3046875" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
-    <col min="4" max="4" width="41.69140625" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
     <col min="5" max="5" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B1" s="69" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.4">
-      <c r="B2" s="70" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:5">
+      <c r="B1" s="65" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+    </row>
+    <row r="2" spans="2:5">
+      <c r="B2" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+    </row>
+    <row r="4" spans="2:5">
       <c r="B4" s="10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.4">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:5">
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:5">
       <c r="B7" s="3"/>
       <c r="C7" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>

</xml_diff>